<commit_message>
fix bug nomor tabel
</commit_message>
<xml_diff>
--- a/DesaKel-Kec.xlsx
+++ b/DesaKel-Kec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\kcda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECT\kcda-blanko-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3826EE-A4A2-4228-ABA7-8E85BA61A24F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331FB68F-9BBB-4042-AA47-D4C6F01CBD15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="202">
   <si>
     <t>Jumlah RW</t>
   </si>
@@ -547,9 +547,6 @@
   </si>
   <si>
     <t>Jumlah Tenaga Kesehatan Menurut Kelurahan/Desa di Kecamatan. 2020</t>
-  </si>
-  <si>
-    <t>Tabel 4.3.2</t>
   </si>
   <si>
     <t>Jumlah Moda Transportasi Laut Menurut Jenis dan  Desa/Kelurahan di Kecamatan, 2020</t>
@@ -704,8 +701,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -880,7 +877,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -938,6 +935,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -947,12 +980,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -962,27 +989,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -992,12 +998,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1005,9 +1005,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1327,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,56 +1339,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="E3" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="F3" s="34" t="s">
+      <c r="E3" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="F3" s="31" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="35"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -1402,13 +1399,13 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>103</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1444,7 +1441,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="26" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -1462,7 +1459,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="25"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5" t="s">
@@ -1476,13 +1473,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="26" t="s">
         <v>158</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="28" t="s">
         <v>102</v>
       </c>
       <c r="D10" s="10" t="s">
@@ -1496,11 +1493,11 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="24"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>103</v>
@@ -1510,7 +1507,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="25"/>
       <c r="C12" s="4"/>
       <c r="D12" s="10" t="s">
@@ -1524,7 +1521,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="25"/>
       <c r="C13" s="4"/>
       <c r="D13" s="10" t="s">
@@ -1538,7 +1535,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="26" t="s">
         <v>72</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -1556,7 +1553,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="25"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5" t="s">
@@ -1570,7 +1567,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="25"/>
       <c r="C16" s="4"/>
       <c r="D16" s="10" t="s">
@@ -1584,7 +1581,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="25"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5" t="s">
@@ -1598,7 +1595,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="25"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5" t="s">
@@ -1612,11 +1609,11 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="25"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>103</v>
@@ -1626,7 +1623,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="26" t="s">
         <v>73</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -1644,7 +1641,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="25"/>
       <c r="C21" s="4"/>
       <c r="D21" s="5" t="s">
@@ -1682,7 +1679,7 @@
       <c r="B23" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="28" t="s">
         <v>104</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -1698,7 +1695,7 @@
     <row r="24" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="25"/>
-      <c r="C24" s="24"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="10" t="s">
         <v>12</v>
       </c>
@@ -1718,7 +1715,7 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>103</v>
@@ -1734,7 +1731,7 @@
       <c r="B26" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="28" t="s">
         <v>112</v>
       </c>
       <c r="D26" s="6" t="s">
@@ -1750,7 +1747,7 @@
     <row r="27" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="24"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="10" t="s">
         <v>15</v>
       </c>
@@ -1768,7 +1765,7 @@
       <c r="B28" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="28" t="s">
         <v>113</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -1784,7 +1781,7 @@
     <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="25"/>
-      <c r="C29" s="24"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="10" t="s">
         <v>15</v>
       </c>
@@ -1802,7 +1799,7 @@
       <c r="B30" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="28" t="s">
         <v>114</v>
       </c>
       <c r="D30" s="6" t="s">
@@ -1818,7 +1815,7 @@
     <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="25"/>
-      <c r="C31" s="24"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="10" t="s">
         <v>15</v>
       </c>
@@ -1836,7 +1833,7 @@
       <c r="B32" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="28" t="s">
         <v>115</v>
       </c>
       <c r="D32" s="6" t="s">
@@ -1852,7 +1849,7 @@
     <row r="33" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="25"/>
-      <c r="C33" s="24"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="10" t="s">
         <v>15</v>
       </c>
@@ -1998,10 +1995,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="33" t="s">
         <v>141</v>
       </c>
       <c r="C43" s="4"/>
@@ -2016,8 +2013,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="4"/>
       <c r="D44" s="6" t="s">
         <v>24</v>
@@ -2030,8 +2027,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="4"/>
       <c r="D45" s="6" t="s">
         <v>25</v>
@@ -2044,10 +2041,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="B46" s="21" t="s">
+      <c r="A46" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="33" t="s">
         <v>141</v>
       </c>
       <c r="C46" s="4"/>
@@ -2062,8 +2059,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="22"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="34"/>
       <c r="C47" s="4"/>
       <c r="D47" s="6" t="s">
         <v>27</v>
@@ -2076,8 +2073,8 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="23"/>
+      <c r="A48" s="35"/>
+      <c r="B48" s="35"/>
       <c r="C48" s="4"/>
       <c r="D48" s="6" t="s">
         <v>28</v>
@@ -2344,13 +2341,13 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="21" t="s">
+      <c r="A66" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="B66" s="21" t="s">
+      <c r="B66" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="36" t="s">
         <v>46</v>
       </c>
       <c r="D66" s="10" t="s">
@@ -2364,9 +2361,9 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="22"/>
-      <c r="B67" s="22"/>
-      <c r="C67" s="27"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="34"/>
+      <c r="C67" s="37"/>
       <c r="D67" s="10" t="s">
         <v>43</v>
       </c>
@@ -2378,13 +2375,13 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="21" t="s">
+      <c r="A68" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="B68" s="21" t="s">
+      <c r="B68" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="C68" s="26" t="s">
+      <c r="C68" s="36" t="s">
         <v>46</v>
       </c>
       <c r="D68" s="10" t="s">
@@ -2398,9 +2395,9 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="22"/>
-      <c r="B69" s="22"/>
-      <c r="C69" s="27"/>
+      <c r="A69" s="34"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="37"/>
       <c r="D69" s="10" t="s">
         <v>45</v>
       </c>
@@ -2412,9 +2409,9 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="27"/>
+      <c r="A70" s="34"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="37"/>
       <c r="D70" s="10" t="s">
         <v>47</v>
       </c>
@@ -2426,9 +2423,9 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="22"/>
-      <c r="B71" s="22"/>
-      <c r="C71" s="27"/>
+      <c r="A71" s="34"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="37"/>
       <c r="D71" s="10" t="s">
         <v>48</v>
       </c>
@@ -2440,9 +2437,9 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="22"/>
-      <c r="B72" s="22"/>
-      <c r="C72" s="27"/>
+      <c r="A72" s="34"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="37"/>
       <c r="D72" s="10" t="s">
         <v>49</v>
       </c>
@@ -2454,9 +2451,9 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
-      <c r="B73" s="23"/>
-      <c r="C73" s="28"/>
+      <c r="A73" s="35"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="38"/>
       <c r="D73" s="10" t="s">
         <v>28</v>
       </c>
@@ -2474,8 +2471,8 @@
       <c r="B74" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C74" s="24" t="s">
-        <v>177</v>
+      <c r="C74" s="28" t="s">
+        <v>176</v>
       </c>
       <c r="D74" s="10" t="s">
         <v>120</v>
@@ -2490,7 +2487,7 @@
     <row r="75" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="25"/>
       <c r="B75" s="25"/>
-      <c r="C75" s="24"/>
+      <c r="C75" s="28"/>
       <c r="D75" s="10" t="s">
         <v>121</v>
       </c>
@@ -2504,7 +2501,7 @@
     <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="25"/>
       <c r="B76" s="25"/>
-      <c r="C76" s="24"/>
+      <c r="C76" s="28"/>
       <c r="D76" s="10" t="s">
         <v>122</v>
       </c>
@@ -2658,10 +2655,10 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="21" t="s">
+      <c r="A86" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="B86" s="21" t="s">
+      <c r="B86" s="33" t="s">
         <v>152</v>
       </c>
       <c r="C86" s="4"/>
@@ -2676,8 +2673,8 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="22"/>
-      <c r="B87" s="22"/>
+      <c r="A87" s="34"/>
+      <c r="B87" s="34"/>
       <c r="C87" s="4"/>
       <c r="D87" s="10" t="s">
         <v>60</v>
@@ -2690,8 +2687,8 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="23"/>
-      <c r="B88" s="23"/>
+      <c r="A88" s="35"/>
+      <c r="B88" s="35"/>
       <c r="C88" s="4"/>
       <c r="D88" s="10" t="s">
         <v>61</v>
@@ -2728,11 +2725,11 @@
       <c r="B90" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C90" s="24" t="s">
+      <c r="C90" s="28" t="s">
         <v>63</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>103</v>
@@ -2744,9 +2741,9 @@
     <row r="91" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="25"/>
       <c r="B91" s="25"/>
-      <c r="C91" s="24"/>
+      <c r="C91" s="28"/>
       <c r="D91" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>103</v>
@@ -2758,9 +2755,9 @@
     <row r="92" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="25"/>
       <c r="B92" s="25"/>
-      <c r="C92" s="24"/>
+      <c r="C92" s="28"/>
       <c r="D92" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>103</v>
@@ -2772,11 +2769,11 @@
     <row r="93" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="25"/>
       <c r="B93" s="25"/>
-      <c r="C93" s="24" t="s">
+      <c r="C93" s="28" t="s">
         <v>64</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>103</v>
@@ -2788,9 +2785,9 @@
     <row r="94" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="25"/>
       <c r="B94" s="25"/>
-      <c r="C94" s="24"/>
+      <c r="C94" s="28"/>
       <c r="D94" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>103</v>
@@ -2802,9 +2799,9 @@
     <row r="95" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="25"/>
       <c r="B95" s="25"/>
-      <c r="C95" s="24"/>
+      <c r="C95" s="28"/>
       <c r="D95" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>103</v>
@@ -2816,11 +2813,11 @@
     <row r="96" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="25"/>
       <c r="B96" s="25"/>
-      <c r="C96" s="24" t="s">
+      <c r="C96" s="28" t="s">
         <v>65</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>103</v>
@@ -2832,9 +2829,9 @@
     <row r="97" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="25"/>
       <c r="B97" s="25"/>
-      <c r="C97" s="24"/>
+      <c r="C97" s="28"/>
       <c r="D97" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>103</v>
@@ -2846,9 +2843,9 @@
     <row r="98" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="25"/>
       <c r="B98" s="25"/>
-      <c r="C98" s="24"/>
+      <c r="C98" s="28"/>
       <c r="D98" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>103</v>
@@ -2866,7 +2863,7 @@
       </c>
       <c r="C99" s="4"/>
       <c r="D99" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>103</v>
@@ -2876,77 +2873,77 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="21" t="s">
+      <c r="A100" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="B100" s="21" t="s">
+      <c r="B100" s="33" t="s">
         <v>155</v>
       </c>
       <c r="C100" s="4"/>
       <c r="D100" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E100" s="7" t="s">
         <v>103</v>
       </c>
       <c r="F100" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="22"/>
-      <c r="B101" s="22"/>
+      <c r="A101" s="34"/>
+      <c r="B101" s="34"/>
       <c r="C101" s="4"/>
       <c r="D101" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>103</v>
       </c>
       <c r="F101" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="22"/>
-      <c r="B102" s="22"/>
+      <c r="A102" s="34"/>
+      <c r="B102" s="34"/>
       <c r="C102" s="4"/>
       <c r="D102" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>103</v>
       </c>
       <c r="F102" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="22"/>
-      <c r="B103" s="22"/>
+      <c r="A103" s="34"/>
+      <c r="B103" s="34"/>
       <c r="C103" s="4"/>
       <c r="D103" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>103</v>
       </c>
       <c r="F103" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="23"/>
-      <c r="B104" s="23"/>
+      <c r="A104" s="35"/>
+      <c r="B104" s="35"/>
       <c r="C104" s="4"/>
       <c r="D104" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>103</v>
       </c>
       <c r="F104" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -3010,11 +3007,11 @@
       </c>
     </row>
     <row r="109" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="21" t="s">
+      <c r="A109" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="B109" s="21" t="s">
-        <v>161</v>
+      <c r="B109" s="33" t="s">
+        <v>160</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="10" t="s">
@@ -3028,8 +3025,8 @@
       </c>
     </row>
     <row r="110" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="22"/>
-      <c r="B110" s="22"/>
+      <c r="A110" s="34"/>
+      <c r="B110" s="34"/>
       <c r="C110" s="4"/>
       <c r="D110" s="10" t="s">
         <v>70</v>
@@ -3042,8 +3039,8 @@
       </c>
     </row>
     <row r="111" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="22"/>
-      <c r="B111" s="22"/>
+      <c r="A111" s="34"/>
+      <c r="B111" s="34"/>
       <c r="C111" s="4"/>
       <c r="D111" s="10" t="s">
         <v>71</v>
@@ -3056,8 +3053,8 @@
       </c>
     </row>
     <row r="112" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="23"/>
-      <c r="B112" s="23"/>
+      <c r="A112" s="35"/>
+      <c r="B112" s="35"/>
       <c r="C112" s="4"/>
       <c r="D112" s="10" t="s">
         <v>41</v>
@@ -3078,17 +3075,80 @@
       </c>
       <c r="C113" s="4"/>
       <c r="D113" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F113" s="14" t="s">
         <v>195</v>
-      </c>
-      <c r="E113" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F113" s="14" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="79">
+    <mergeCell ref="A109:A112"/>
+    <mergeCell ref="B109:B112"/>
+    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="A90:A98"/>
+    <mergeCell ref="B90:B98"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="B100:B104"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="C93:C95"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="C90:C92"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="B68:B73"/>
+    <mergeCell ref="C68:C73"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="A58:A62"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="B49:B53"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B14:B19"/>
     <mergeCell ref="A14:A19"/>
@@ -3105,69 +3165,6 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="B49:B53"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="A58:A62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="A68:A73"/>
-    <mergeCell ref="B68:B73"/>
-    <mergeCell ref="C68:C73"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="C90:C92"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="A109:A112"/>
-    <mergeCell ref="B109:B112"/>
-    <mergeCell ref="C96:C98"/>
-    <mergeCell ref="A90:A98"/>
-    <mergeCell ref="B90:B98"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="B100:B104"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="C93:C95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId1"/>
@@ -3193,61 +3190,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38" t="s">
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="12">
         <v>2020</v>
       </c>
@@ -3272,18 +3269,18 @@
       <c r="K4" s="12">
         <v>2013</v>
       </c>
-      <c r="L4" s="38"/>
+      <c r="L4" s="41"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>164</v>
-      </c>
       <c r="D5" s="7" t="s">
         <v>103</v>
       </c>
@@ -3308,7 +3305,7 @@
       <c r="K5" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="39">
+      <c r="L5" s="21">
         <v>3</v>
       </c>
     </row>
@@ -3316,7 +3313,7 @@
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>103</v>
@@ -3342,7 +3339,7 @@
       <c r="K6" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="39">
+      <c r="L6" s="21">
         <v>1</v>
       </c>
     </row>
@@ -3350,7 +3347,7 @@
       <c r="A7" s="25"/>
       <c r="B7" s="25"/>
       <c r="C7" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>103</v>
@@ -3376,19 +3373,19 @@
       <c r="K7" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>168</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>169</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>103</v>
@@ -3400,15 +3397,15 @@
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
-      <c r="L8" s="40" t="s">
-        <v>172</v>
+      <c r="L8" s="22" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="44" t="s">
-        <v>170</v>
+      <c r="A9" s="43"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="23" t="s">
+        <v>169</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>103</v>
@@ -3420,15 +3417,15 @@
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="39">
+      <c r="L9" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="44" t="s">
-        <v>171</v>
+      <c r="A10" s="43"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="23" t="s">
+        <v>170</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>103</v>
@@ -3440,14 +3437,14 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="39">
+      <c r="L10" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="44" t="s">
+      <c r="A11" s="43"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -3460,14 +3457,14 @@
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
-      <c r="L11" s="39">
+      <c r="L11" s="21">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="44" t="s">
+      <c r="A12" s="44"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -3480,12 +3477,14 @@
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
-      <c r="L12" s="39">
+      <c r="L12" s="21">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A1:L1"/>
@@ -3494,8 +3493,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:K3"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>